<commit_message>
Improve output format with single serial numbers column
Changed output to have a single "Assigned Serial Numbers" column instead
of separate columns per card type. The format is now:

  Choices $200: SN1, SN2; Save-On $50: SN3; Save-On $200: SN4,SN5

This makes it much easier to read in Excel, with all information in one
column. Labels are shortened (e.g., "Choices Market" -> "Choices") for
better readability. The column is automatically widened to 80 chars.

Updated tests to match new output format.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
Co-authored-by: Sculptor <sculptor@imbue.com>
</commit_message>
<xml_diff>
--- a/test_data/assigned_envelopes.xlsx
+++ b/test_data/assigned_envelopes.xlsx
@@ -426,13 +426,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="80" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -447,37 +450,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Choices Market $100</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Choices Market $200</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Save-On-Foods $100</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Save-On-Foods $200</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Save-On-Foods $50</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Urban Fare $100</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Urban Fare $50</t>
+          <t>Assigned Serial Numbers</t>
         </is>
       </c>
     </row>
@@ -490,17 +463,11 @@
           <t>Hosen-Töter, Campino</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>6275330202500880384 6275330202500880384 6275330202500880384 6275330202500880384 6275330202500880384 6275330202500880384 6275330202500880384 6275330202500880384 6275330202500880384 6275330202500880384</t>
+          <t>Choices $200: 6275330202500880384, 6275330202500880384, 6275330202500880384, 6275330202500880384, 6275330202500880384, 6275330202500880384, 6275330202500880384, 6275330202500880384, 6275330202500880384, 6275330202500880384</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>